<commit_message>
IG: masnick/core-ig, ref: patch-1  run_id: 6383419545, run_number: 16, run_attempt: 1 with branch SHA: 0c92b8985fced75dfc78bdd6978733e2c0bea676 and merge SHA: c074acd313bfe79aadf8fa1452ebd78d631c37fb
</commit_message>
<xml_diff>
--- a/ig/pull/92_FROM_masnick_core-ig_patch-1_TO_master/CodeSystem-HtsFormat.xlsx
+++ b/ig/pull/92_FROM_masnick_core-ig_patch-1_TO_master/CodeSystem-HtsFormat.xlsx
@@ -281,10 +281,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>